<commit_message>
arbitrage and EV betting update
</commit_message>
<xml_diff>
--- a/final visualizations/roi_table.xlsx
+++ b/final visualizations/roi_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joepopop/Desktop/Data Science Projects/soccer_betting_simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joepopop/Desktop/Data Science Projects/soccer_betting_simulation/final visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A10D34-8E33-2F43-8ACC-2B0B7A3FF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC7731-AE43-FE47-A5BE-56872E7E655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{4558F208-BF14-7046-937E-199514D0BC51}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ROI</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>Aribitrage</t>
-  </si>
-  <si>
     <t>Nearest Neighbors</t>
   </si>
   <si>
@@ -89,6 +86,15 @@
   </si>
   <si>
     <t>Random Forest (A&amp;D)</t>
+  </si>
+  <si>
+    <t>Positive EV (4%)</t>
+  </si>
+  <si>
+    <t>Arbitrage</t>
+  </si>
+  <si>
+    <t>Arbitrage (Compounded)</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -185,6 +191,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,8 +230,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8CB357D-02FA-7549-A05B-774A2FCB275A}" name="Table1" displayName="Table1" ref="E1:J13" totalsRowShown="0">
-  <autoFilter ref="E1:J13" xr:uid="{C8CB357D-02FA-7549-A05B-774A2FCB275A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8CB357D-02FA-7549-A05B-774A2FCB275A}" name="Table1" displayName="Table1" ref="E1:J15" totalsRowShown="0">
+  <autoFilter ref="E1:J15" xr:uid="{C8CB357D-02FA-7549-A05B-774A2FCB275A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:J11">
     <sortCondition descending="1" ref="I1:I11"/>
   </sortState>
@@ -541,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0A8D06-F4D2-5646-85CF-B0EFB65930B3}">
-  <dimension ref="E1:J13"/>
+  <dimension ref="E1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,7 +559,9 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="3.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,7 +576,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -578,32 +587,33 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F11" si="0">G2/(I2*J2)</f>
-        <v>9.5000000000000015E-3</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="8">
+        <f>G2/(I2*J2)</f>
+        <v>6.9493541247484907E-3</v>
       </c>
       <c r="G2">
-        <v>67.260000000000005</v>
+        <f>3.453829</f>
+        <v>3.4538289999999998</v>
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Matches]]*Table1[[#This Row],[Cost per match]]</f>
-        <v>7080</v>
+        <v>497</v>
       </c>
       <c r="I2">
-        <v>2360</v>
+        <v>497</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F3:F11" si="0">G3/(I3*J3)</f>
         <v>2.3574257425742574E-2</v>
       </c>
       <c r="G3">
@@ -622,7 +632,7 @@
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
@@ -644,7 +654,7 @@
     </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
@@ -666,7 +676,7 @@
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
@@ -688,7 +698,7 @@
     </row>
     <row r="7" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
@@ -710,7 +720,7 @@
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
@@ -732,7 +742,7 @@
     </row>
     <row r="9" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
@@ -754,7 +764,7 @@
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
@@ -776,7 +786,7 @@
     </row>
     <row r="11" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
@@ -798,7 +808,7 @@
     </row>
     <row r="12" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1">
         <f>G12/(I12*J12)</f>
@@ -820,7 +830,7 @@
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="1">
         <f>G13/(I13*J13)</f>
@@ -837,6 +847,50 @@
         <v>436</v>
       </c>
       <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1">
+        <f>G14/(I14*J14)</f>
+        <v>-2.8248648648648646E-2</v>
+      </c>
+      <c r="G14">
+        <v>-26.13</v>
+      </c>
+      <c r="H14">
+        <f>Table1[[#This Row],[Matches]]*Table1[[#This Row],[Cost per match]]</f>
+        <v>925</v>
+      </c>
+      <c r="I14">
+        <v>925</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1">
+        <f>G15/(I15*J15)</f>
+        <v>6.4702849899999998E-2</v>
+      </c>
+      <c r="G15">
+        <v>3.2351424949999998</v>
+      </c>
+      <c r="H15">
+        <f>Table1[[#This Row],[Matches]]*Table1[[#This Row],[Cost per match]]</f>
+        <v>50</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15">
         <v>1</v>
       </c>
     </row>

</xml_diff>